<commit_message>
Add formuls for counting hours in plane
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>Шапка РУП</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>ПЛАН*</t>
+  </si>
+  <si>
+    <t>R4138</t>
+  </si>
+  <si>
+    <t>R3234</t>
   </si>
   <si>
     <t>Иностранный язык в профессиональной деятельности</t>
@@ -515,8 +521,6 @@
     <col customWidth="1" max="1" min="1" width="81.59999999999999"/>
     <col customWidth="1" max="2" min="2" width="21.6"/>
     <col customWidth="1" max="3" min="3" width="8.4"/>
-    <col customWidth="1" max="4" min="4" width="9.6"/>
-    <col customWidth="1" max="5" min="5" width="7.199999999999999"/>
     <col customWidth="1" max="6" min="6" width="7.199999999999999"/>
     <col customWidth="1" max="7" min="7" width="7.199999999999999"/>
     <col customWidth="1" max="8" min="8" width="7.199999999999999"/>
@@ -3532,8 +3536,12 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="F3" s="1" t="n"/>
       <c r="G3" s="1" t="n"/>
       <c r="H3" s="1" t="n"/>
@@ -4532,266 +4540,458 @@
     </row>
     <row r="4" spans="1:1000">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>34</v>
+      </c>
+      <c r="D4" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A4,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B4</f>
+        <v/>
+      </c>
+      <c r="E4" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A4,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B4</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:1000">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A5,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B5</f>
+        <v/>
+      </c>
+      <c r="E5" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A5,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B5</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:1000">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A6,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B6</f>
+        <v/>
+      </c>
+      <c r="E6" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A6,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B6</f>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:1000">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="D7" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A7,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B7</f>
+        <v/>
+      </c>
+      <c r="E7" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A7,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B7</f>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:1000">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A8,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B8</f>
+        <v/>
+      </c>
+      <c r="E8" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A8,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B8</f>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:1000">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="D9" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A9,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B9</f>
+        <v/>
+      </c>
+      <c r="E9" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A9,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B9</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:1000">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>84</v>
+      </c>
+      <c r="D10" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A10,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B10</f>
+        <v/>
+      </c>
+      <c r="E10" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A10,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B10</f>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:1000">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A11,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B11</f>
+        <v/>
+      </c>
+      <c r="E11" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A11,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B11</f>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:1000">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="D12" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A12,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B12</f>
+        <v/>
+      </c>
+      <c r="E12" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A12,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B12</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:1000">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>30</v>
+      </c>
+      <c r="D13" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A13,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B13</f>
+        <v/>
+      </c>
+      <c r="E13" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A13,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B13</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:1000">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A14,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B14</f>
+        <v/>
+      </c>
+      <c r="E14" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A14,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B14</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:1000">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="D15" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A15,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B15</f>
+        <v/>
+      </c>
+      <c r="E15" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A15,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B15</f>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:1000">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>30</v>
+      </c>
+      <c r="D16" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A16,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B16</f>
+        <v/>
+      </c>
+      <c r="E16" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A16,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B16</f>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:1000">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A17,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B17</f>
+        <v/>
+      </c>
+      <c r="E17" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A17,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B17</f>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:1000">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="D18" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A18,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B18</f>
+        <v/>
+      </c>
+      <c r="E18" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A18,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B18</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:1000">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>30</v>
+      </c>
+      <c r="D19" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A19,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B19</f>
+        <v/>
+      </c>
+      <c r="E19" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A19,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B19</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:1000">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A20,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B20</f>
+        <v/>
+      </c>
+      <c r="E20" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A20,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B20</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:1000">
       <c r="A21" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="D21" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A21,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B21</f>
+        <v/>
+      </c>
+      <c r="E21" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A21,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B21</f>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:1000">
       <c r="A22" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>34</v>
+      </c>
+      <c r="D22" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A22,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B22</f>
+        <v/>
+      </c>
+      <c r="E22" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A22,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B22</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:1000">
       <c r="A23" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="D23" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A23,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B23</f>
+        <v/>
+      </c>
+      <c r="E23" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A23,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B23</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:1000">
       <c r="A24" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>42</v>
+      </c>
+      <c r="D24" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A24,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B24</f>
+        <v/>
+      </c>
+      <c r="E24" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A24,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B24</f>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:1000">
       <c r="A25" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A25,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B25</f>
+        <v/>
+      </c>
+      <c r="E25" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A25,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B25</f>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:1000">
       <c r="A26" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="D26" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A26,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B26</f>
+        <v/>
+      </c>
+      <c r="E26" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A26,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B26</f>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:1000">
       <c r="A27" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A27,Расписание!$I$2:$I$10000,'Сводная страница'!D$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B27</f>
+        <v/>
+      </c>
+      <c r="E27" s="2">
+        <f>2*COUNTIFS(Расписание!$E$2:$E$10000,'Сводная страница'!$A27,Расписание!$I$2:$I$10000,'Сводная страница'!E$3,Расписание!$F$2:$F$10000,'Сводная страница'!$B27</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -5820,31 +6020,31 @@
   <sheetData>
     <row r="1" spans="1:1000">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
@@ -7861,7 +8061,7 @@
   <sheetData>
     <row r="1" spans="1:1000">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="n"/>
       <c r="C1" s="1" t="n"/>
@@ -8865,21 +9065,21 @@
     </row>
     <row r="2" spans="1:1000">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row customHeight="1" ht="30" r="3" spans="1:1000">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1000"/>
     <row r="5" spans="1:1000">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="n"/>
       <c r="D5" s="1" t="n"/>
@@ -9882,58 +10082,58 @@
     </row>
     <row r="6" spans="1:1000">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:1000">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1000">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:1000">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:1000">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:1000">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:1000">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>